<commit_message>
TP1 VERSION FINAL 2
</commit_message>
<xml_diff>
--- a/TPs/TP1_Jugando con APIS y Webscrapping/TP1 Uba punto N.xlsx
+++ b/TPs/TP1_Jugando con APIS y Webscrapping/TP1 Uba punto N.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B159"/>
+  <dimension ref="A1:B160"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -536,7 +536,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/la-oficina-del-presidente-repudio-el-rechazo-de-los-pliegos-de-lijo-y-garcia-mansilla-en-el-senado-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/el-juez-ramos-padilla-ordeno-que-garcia-mansilla-se-abstenga-de-tomar-decisiones-en-la-corte-suprema-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -546,7 +546,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/la-opinion-mayoritaria-de-los-constitucionalistas-es-que-garcia-mansilla-debe-dejar-de-inmediato-la-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/la-oficina-del-presidente-repudio-el-rechazo-de-los-pliegos-de-lijo-y-garcia-mansilla-en-el-senado-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -556,7 +556,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/duro-cruce-de-la-casa-rosada-a-victoria-villarruel-tras-los-intentos-fallidos-por-evitar-la-sesion-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/la-opinion-mayoritaria-de-los-constitucionalistas-es-que-garcia-mansilla-debe-dejar-de-inmediato-la-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -636,7 +636,7 @@
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/anabel-fernandez-sagasti-acuso-a-lorenzetti-de-amenazar-al-kirchnerismo-con-meter-presa-a-cristina-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/garcia-mansilla-se-prepara-para-quedarse-en-la-corte-sostenido-por-el-gobierno-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -646,7 +646,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/desconcertada-europa-promete-responder-a-los-aranceles-de-trump-pero-se-abre-a-negociar-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/anabel-fernandez-sagasti-acuso-a-lorenzetti-de-amenazar-al-kirchnerismo-con-meter-presa-a-cristina-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -656,7 +656,7 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/dia-de-la-liberacion-o-dia-de-la-destruccion-trump-abre-una-nueva-era-global-plagada-de-incognitas-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/desconcertada-europa-promete-responder-a-los-aranceles-de-trump-pero-se-abre-a-negociar-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -666,7 +666,7 @@
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/los-aranceles-de-trump-profundizan-el-abismo-entre-eeuu-y-sus-aliados-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/dia-de-la-liberacion-o-dia-de-la-destruccion-trump-abre-una-nueva-era-global-plagada-de-incognitas-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -676,7 +676,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/aranceles-de-trump-la-soja-termino-en-rojo-en-los-estados-unidos-y-en-la-argentina-la-nueva-cosecha-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/los-aranceles-de-trump-profundizan-el-abismo-entre-eeuu-y-sus-aliados-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/el-gobierno-quiere-acelerar-la-privatizacion-de-corredores-viales-con-una-intervencion-que-podria-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/aranceles-de-trump-la-soja-termino-en-rojo-en-los-estados-unidos-y-en-la-argentina-la-nueva-cosecha-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -696,7 +696,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/aerolineas-argentinas-tuvo-ganancias-por-primera-vez-desde-la-estatizacion-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/el-gobierno-quiere-acelerar-la-privatizacion-de-corredores-viales-con-una-intervencion-que-podria-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -706,7 +706,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/cultura/el-gobierno-no-le-renovo-el-contrato-al-fotografo-que-saco-la-foto-al-cabo-que-hirio-a-pablo-grillo-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/aerolineas-argentinas-tuvo-ganancias-por-primera-vez-desde-la-estatizacion-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -716,7 +716,7 @@
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/boca-presento-su-nueva-camiseta-alternativa-en-su-120-aniversario-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/cultura/el-gobierno-no-le-renovo-el-contrato-al-fotografo-que-saco-la-foto-al-cabo-que-hirio-a-pablo-grillo-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/tras-su-discurso-por-el-2-de-abril-declaran-persona-no-grata-a-javier-milei-en-ushuaia-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/deportes/boca-presento-su-nueva-camiseta-alternativa-en-su-120-aniversario-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -736,7 +736,7 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sociedad/caos-en-palermo-por-el-show-gratuito-de-tini-stoessel-peleas-entre-fanaticas-y-quejas-de-los-vecinos-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/tras-su-discurso-por-el-2-de-abril-declaran-persona-no-grata-a-javier-milei-en-ushuaia-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -746,7 +746,7 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/la-oficina-del-presidente-repudio-el-rechazo-de-los-pliegos-de-lijo-y-garcia-mansilla-en-el-senado-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/sociedad/caos-en-palermo-por-el-show-gratuito-de-tini-stoessel-peleas-entre-fanaticas-y-quejas-de-los-vecinos-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -756,7 +756,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/garcia-mansilla-se-prepara-para-quedarse-en-la-corte-sostenido-por-el-gobierno-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/la-oficina-del-presidente-repudio-el-rechazo-de-los-pliegos-de-lijo-y-garcia-mansilla-en-el-senado-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -766,7 +766,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/la-relacion-con-trump-comenzo-una-hermetica-negociacion-para-que-vengan-toros-y-vacas-de-estados-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/el-juez-ramos-padilla-ordeno-que-garcia-mansilla-se-abstenga-de-tomar-decisiones-en-la-corte-suprema-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -776,7 +776,7 @@
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/javier-milei-en-vivo-las-ultimas-medidas-del-gobierno-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/garcia-mansilla-se-prepara-para-quedarse-en-la-corte-sostenido-por-el-gobierno-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -786,7 +786,7 @@
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/seguridad/la-disputa-familiar-por-la-marca-maradona-exploto-en-el-juicio-por-la-muerte-del-astro-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/la-relacion-con-trump-comenzo-una-hermetica-negociacion-para-que-vengan-toros-y-vacas-de-estados-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -796,7 +796,7 @@
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/caballito-el-secreto-del-barrio-que-siempre-sorprende-y-el-despegue-de-una-microzona-trendy-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/seguridad/la-disputa-familiar-por-la-marca-maradona-exploto-en-el-juicio-por-la-muerte-del-astro-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/la-argentina-tuvo-una-leve-caida-de-la-desigualdad-al-final-de-2024-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/propiedades/caballito-el-secreto-del-barrio-que-siempre-sorprende-y-el-despegue-de-una-microzona-trendy-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -816,7 +816,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/la-historia-desconocida-de-paladium-el-otro-dueno-la-foto-que-desperto-el-interes-de-su-hijo-y-el-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/la-argentina-tuvo-una-leve-caida-de-la-desigualdad-al-final-de-2024-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -826,7 +826,7 @@
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/javier-milei-llego-a-estados-unidos-y-busca-su-foto-con-donald-trump-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/la-historia-desconocida-de-paladium-el-otro-dueno-la-foto-que-desperto-el-interes-de-su-hijo-y-el-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -836,7 +836,7 @@
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/los-aranceles-de-trump-la-mesa-de-enlace-le-transmitio-su-inquietud-al-gobierno-y-pidio-analizar-el-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/javier-milei-llego-a-estados-unidos-y-busca-su-foto-con-donald-trump-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -846,7 +846,7 @@
       </c>
       <c r="B42" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/jorge-macri-acuso-a-manuel-adorni-de-no-conocer-a-la-ciudad-y-el-vocero-le-respondio-con-una-chicana-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/los-aranceles-de-trump-la-mesa-de-enlace-le-transmitio-su-inquietud-al-gobierno-y-pidio-analizar-el-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -856,7 +856,7 @@
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/un-ajedrez-inesperado-en-la-lucha-por-el-poder-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/politica/jorge-macri-acuso-a-manuel-adorni-de-no-conocer-a-la-ciudad-y-el-vocero-le-respondio-con-una-chicana-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -866,7 +866,7 @@
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/cultura/santiago-caputo-es-el-monje-desde-la-tia-ines-y-la-primera-cita-con-duran-barba-un-curriculum-que-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/un-ajedrez-inesperado-en-la-lucha-por-el-poder-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -876,7 +876,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/negocios/el-pais-que-casi-expulsan-de-la-union-europea-y-se-recupera-de-a-poco-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/cultura/santiago-caputo-es-el-monje-desde-la-tia-ines-y-la-primera-cita-con-duran-barba-un-curriculum-que-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -886,7 +886,7 @@
       </c>
       <c r="B46" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/tenis/maradona-en-moscu-el-hincha-fervoroso-las-noches-agitadas-con-alcohol-y-el-top-ten-con-un-doberman-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/negocios/el-pais-que-casi-expulsan-de-la-union-europea-y-se-recupera-de-a-poco-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -896,7 +896,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/juan-verdaguer-un-violin-una-escalera-y-las-invisibles-herramientas-de-un-humorista-unico-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/deportes/tenis/maradona-en-moscu-el-hincha-fervoroso-las-noches-agitadas-con-alcohol-y-el-top-ten-con-un-doberman-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -906,7 +906,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/futbol/el-atletico-de-madrid-de-cholo-simeone-y-varios-campeones-mundiales-de-todo-a-casi-nada-en-25-dias-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/juan-verdaguer-un-violin-una-escalera-y-las-invisibles-herramientas-de-un-humorista-unico-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -916,7 +916,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/futbol/boca-cumple-120-anos-mitos-y-verdades-de-su-fundacion-libro-especial-y-camiseta-nueva-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/el-atletico-de-madrid-de-cholo-simeone-y-varios-campeones-mundiales-de-todo-a-casi-nada-en-25-dias-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -926,7 +926,7 @@
       </c>
       <c r="B50" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/automovilismo/colapinto-debera-esperar-el-acuerdo-de-alpine-que-ratifica-a-jack-doohan-en-el-gp-de-miami-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/deportes/futbol/boca-cumple-120-anos-mitos-y-verdades-de-su-fundacion-libro-especial-y-camiseta-nueva-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -936,7 +936,7 @@
       </c>
       <c r="B51" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/efecto-ghibli-chatgpt-genero-700-millones-de-imagenes-en-una-semana-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/deportes/automovilismo/colapinto-debera-esperar-el-acuerdo-de-alpine-que-ratifica-a-jack-doohan-en-el-gp-de-miami-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -946,7 +946,7 @@
       </c>
       <c r="B52" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sociedad/adolescentes-el-estres-digital-la-otra-preocupacion-que-suman-las-redes-sociales-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/efecto-ghibli-chatgpt-genero-700-millones-de-imagenes-en-una-semana-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/para-competir-con-starlink-los-primeros-27-satelites-kuiper-de-amazon-iran-al-espacio-este-miercoles-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/sociedad/adolescentes-el-estres-digital-la-otra-preocupacion-que-suman-las-redes-sociales-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -966,7 +966,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/avro-691-lancastrian-un-ataque-terrorista-teorias-extraterrestres-y-un-misterio-que-duro-mas-de-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/para-competir-con-starlink-los-primeros-27-satelites-kuiper-de-amazon-iran-al-espacio-este-miercoles-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -976,7 +976,7 @@
       </c>
       <c r="B55" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/al-volante/como-se-llamara-la-nueva-pickup-de-volkswagen-y-por-que-la-argentina-sera-el-unico-proveedor-de-la-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/avro-691-lancastrian-un-ataque-terrorista-teorias-extraterrestres-y-un-misterio-que-duro-mas-de-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -986,7 +986,7 @@
       </c>
       <c r="B56" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-hola/tiene-56-anos-fue-supermodelo-en-los-90-y-hoy-se-luce-en-otra-faceta-mi-carrera-como-modelo-fue-una-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/autos/al-volante/como-se-llamara-la-nueva-pickup-de-volkswagen-y-por-que-la-argentina-sera-el-unico-proveedor-de-la-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -996,7 +996,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-hola/los-65-de-marcelo-tinelli-todas-las-fotos-y-los-invitados-de-una-super-fiesta-en-las-alturas-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/revista-hola/tiene-56-anos-fue-supermodelo-en-los-90-y-hoy-se-luce-en-otra-faceta-mi-carrera-como-modelo-fue-una-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1006,7 +1006,7 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/raquel-mancini-de-su-vuelta-al-trabajo-a-por-que-se-mudo-con-su-mama-y-quien-es-su-pareja-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/revista-hola/los-65-de-marcelo-tinelli-todas-las-fotos-y-los-invitados-de-una-super-fiesta-en-las-alturas-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1016,7 +1016,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/fue-campeon-en-la-argentina-se-instalo-en-el-sur-de-la-india-y-cumple-su-sueno-me-considero-un-poco-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/raquel-mancini-de-su-vuelta-al-trabajo-a-por-que-se-mudo-con-su-mama-y-quien-es-su-pareja-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1026,7 +1026,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/rosamund-pike-recordo-la-vergonzosa-situacion-que-vivio-mientras-filmaba-una-escena-de-sexo-con-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/deportes/fue-campeon-en-la-argentina-se-instalo-en-el-sur-de-la-india-y-cumple-su-sueno-me-considero-un-poco-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1036,7 +1036,7 @@
       </c>
       <c r="B61" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/no-se-dejaba-tocar-pero-estaba-tan-enferma-que-maullo-hasta-que-ella-entendio-lo-que-necesitaba-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/rosamund-pike-recordo-la-vergonzosa-situacion-que-vivio-mientras-filmaba-una-escena-de-sexo-con-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1046,7 +1046,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/el-pedido-de-ayuda-de-peter-lanzani-y-su-novia-luego-de-sufrir-un-robo-en-neuquen-a-dos-semanas-de-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/no-se-dejaba-tocar-pero-estaba-tan-enferma-que-maullo-hasta-que-ella-entendio-lo-que-necesitaba-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1056,7 +1056,7 @@
       </c>
       <c r="B63" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/mapas-mentales-y-busqueda-de-fuentes-como-notebooklm-la-ia-de-google-te-ayuda-a-estudiar-mejor-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/el-pedido-de-ayuda-de-peter-lanzani-y-su-novia-luego-de-sufrir-un-robo-en-neuquen-a-dos-semanas-de-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1066,7 +1066,7 @@
       </c>
       <c r="B64" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-living/despues-de-anos-de-alquilar-casas-de-vacaciones-en-el-delta-una-disenadora-decidio-construir-la-suya-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/mapas-mentales-y-busqueda-de-fuentes-como-notebooklm-la-ia-de-google-te-ayuda-a-estudiar-mejor-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1076,7 +1076,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/trivias/trivia-exclusiva-cuanto-sabes-sobre-kobe-bryant-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/revista-living/despues-de-anos-de-alquilar-casas-de-vacaciones-en-el-delta-una-disenadora-decidio-construir-la-suya-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1086,7 +1086,7 @@
       </c>
       <c r="B66" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/seguridad/batalla-campal-entre-policias-que-jugaban-un-partido-de-futbol-5-y-fueron-atacados-por-barras-bravas-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/juegos/trivias/trivia-exclusiva-cuanto-sabes-sobre-kobe-bryant-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1096,7 +1096,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/michelle-williams-el-osado-regreso-de-la-actriz-que-se-le-planto-a-hollywood-y-casi-abandona-su-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/seguridad/batalla-campal-entre-policias-que-jugaban-un-partido-de-futbol-5-y-fueron-atacados-por-barras-bravas-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1106,7 +1106,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/usan-ia-para-evaluar-la-edad-del-corazon-y-adelantar-la-deteccion-de-enfermedades-cardiacas-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/michelle-williams-el-osado-regreso-de-la-actriz-que-se-le-planto-a-hollywood-y-casi-abandona-su-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1116,7 +1116,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/una-revista-publico-fotos-de-la-princesa-leonor-en-bikini-en-uruguay-y-genero-revuelo-en-espana-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/usan-ia-para-evaluar-la-edad-del-corazon-y-adelantar-la-deteccion-de-enfermedades-cardiacas-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1126,7 +1126,7 @@
       </c>
       <c r="B70" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/nexos/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/una-revista-publico-fotos-de-la-princesa-leonor-en-bikini-en-uruguay-y-genero-revuelo-en-espana-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1136,7 +1136,7 @@
       </c>
       <c r="B71" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/cruci-tematico/</t>
+          <t>https://www.lanacion.com.ar/juegos/nexos/</t>
         </is>
       </c>
     </row>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/panal-de-letras/</t>
+          <t>https://www.lanacion.com.ar/juegos/cruci-tematico/</t>
         </is>
       </c>
     </row>
@@ -1156,7 +1156,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/sudoku/</t>
+          <t>https://www.lanacion.com.ar/juegos/panal-de-letras/</t>
         </is>
       </c>
     </row>
@@ -1166,7 +1166,7 @@
       </c>
       <c r="B74" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/opinion/scaloni-julio-bocca-y-la-generacion-dorada-tres-cursos-para-la-politica-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/juegos/sudoku/</t>
         </is>
       </c>
     </row>
@@ -1176,7 +1176,7 @@
       </c>
       <c r="B75" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/opinion/malvinas-milei-entre-el-alineamiento-con-trump-el-narcisismo-y-la-improvisacion-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/opinion/scaloni-julio-bocca-y-la-generacion-dorada-tres-cursos-para-la-politica-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1186,7 +1186,7 @@
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/opinion/deepseek-y-medicina-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/opinion/malvinas-milei-entre-el-alineamiento-con-trump-el-narcisismo-y-la-improvisacion-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1196,7 +1196,7 @@
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/editoriales/malvinas-honrar-a-los-heroes-senalar-a-los-mentirosos-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/opinion/deepseek-y-medicina-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1206,7 +1206,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/editoriales/los-25-anos-de-cippec-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/editoriales/malvinas-honrar-a-los-heroes-senalar-a-los-mentirosos-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/la-turbulencia-no-derriba-aviones-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/editoriales/los-25-anos-de-cippec-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1226,7 +1226,7 @@
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/efecto-ghibli-chatgpt-genero-700-millones-de-imagenes-en-una-semana-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/la-turbulencia-no-derriba-aviones-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1236,7 +1236,7 @@
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/IA/un-diario-italiano-publico-un-suplemento-realizado-exclusivamente-con-inteligencia-artificial-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/efecto-ghibli-chatgpt-genero-700-millones-de-imagenes-en-una-semana-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1246,7 +1246,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/innovacion-en-la-nube-cual-es-el-motor-clave-para-la-transformacion-empresarial-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/IA/un-diario-italiano-publico-un-suplemento-realizado-exclusivamente-con-inteligencia-artificial-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1256,7 +1256,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/medida-el-gobierno-realizo-un-fuerte-cambio-en-fertilizantes-y-sturzenegger-sorprendio-con-un-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/innovacion-en-la-nube-cual-es-el-motor-clave-para-la-transformacion-empresarial-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1266,7 +1266,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/dia-de-los-lamentos-muy-volatil-la-soja-baja-tras-los-aranceles-del-dia-de-la-liberacion-de-donald-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/medida-el-gobierno-realizo-un-fuerte-cambio-en-fertilizantes-y-sturzenegger-sorprendio-con-un-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1276,7 +1276,7 @@
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/emplea-a-180-personas-una-empresa-del-agro-reducira-salarios-horas-de-trabajo-y-no-descarta-avanzar-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/dia-de-los-lamentos-muy-volatil-la-soja-baja-tras-los-aranceles-del-dia-de-la-liberacion-de-donald-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1286,7 +1286,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/dia-de-la-liberacion-el-arancel-universal-de-trump-puso-en-alerta-a-decenas-de-exportadores-del-agro-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/emplea-a-180-personas-una-empresa-del-agro-reducira-salarios-horas-de-trabajo-y-no-descarta-avanzar-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/los-10-famosos-con-mas-seguidores-en-instagram-x-y-tiktok-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/dia-de-la-liberacion-el-arancel-universal-de-trump-puso-en-alerta-a-decenas-de-exportadores-del-agro-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1306,7 +1306,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/cuales-son-los-tres-signos-con-menos-suerte-en-abril-2025-segun-la-inteligencia-artificial-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/los-10-famosos-con-mas-seguidores-en-instagram-x-y-tiktok-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1316,7 +1316,7 @@
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/tecnologia/como-activar-el-modo-chavo-del-8-en-whatsapp-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/cuales-son-los-tres-signos-con-menos-suerte-en-abril-2025-segun-la-inteligencia-artificial-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1326,7 +1326,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/cande-molfese-fue-vista-a-los-besos-con-un-misterioso-hombre-y-causo-revuelo-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/tecnologia/como-activar-el-modo-chavo-del-8-en-whatsapp-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1336,7 +1336,7 @@
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/cande-tinelli-conto-la-verdad-detras-de-su-separacion-de-coti-sorokin-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/cande-molfese-fue-vista-a-los-besos-con-un-misterioso-hombre-y-causo-revuelo-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1346,7 +1346,7 @@
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/en-las-redes/crece-la-preocupacion-de-los-cientificos-de-la-nasa-por-una-anomalia-magnetica-en-el-atlantico-sur-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/cande-tinelli-conto-la-verdad-detras-de-su-separacion-de-coti-sorokin-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1356,7 +1356,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/el-inesperado-saludo-de-wanda-nara-a-maxi-lopez-por-su-cumpleanos-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/en-las-redes/crece-la-preocupacion-de-los-cientificos-de-la-nasa-por-una-anomalia-magnetica-en-el-atlantico-sur-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1366,7 +1366,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/en-las-redes/cual-es-tu-carrera-ideal-segun-tu-fecha-de-nacimiento-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/el-inesperado-saludo-de-wanda-nara-a-maxi-lopez-por-su-cumpleanos-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1376,7 +1376,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/cuidado-cuerpo-belleza/los-multiples-beneficios-de-incorporar-las-semillas-de-limon-en-las-comidas-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/en-las-redes/cual-es-tu-carrera-ideal-segun-tu-fecha-de-nacimiento-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1386,7 +1386,7 @@
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/juegos/retos-visuales/desafio-matematico-animate-a-resolverlo-en-solo-10-segundos-y-pone-a-prueba-tu-coeficiente-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/cuidado-cuerpo-belleza/los-multiples-beneficios-de-incorporar-las-semillas-de-limon-en-las-comidas-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1396,7 +1396,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/un-ajedrez-inesperado-en-la-lucha-por-el-poder-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/juegos/retos-visuales/desafio-matematico-animate-a-resolverlo-en-solo-10-segundos-y-pone-a-prueba-tu-coeficiente-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1406,7 +1406,7 @@
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sociedad/la-mugre-se-volvio-parte-del-paisaje-el-impensado-barrio-porteno-que-concentra-las-quejas-por-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/el-mundo/una-revista-publico-fotos-de-la-princesa-leonor-en-bikini-en-uruguay-y-genero-revuelo-en-espana-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1416,7 +1416,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/el-mundo/una-revista-publico-fotos-de-la-princesa-leonor-en-bikini-en-uruguay-y-genero-revuelo-en-espana-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/un-ajedrez-inesperado-en-la-lucha-por-el-poder-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/dolar/guerra-comercial-el-euro-se-revaloriza-a-su-maximo-desde-octubre-tras-los-anuncios-de-donald-trump-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/sociedad/la-mugre-se-volvio-parte-del-paisaje-el-impensado-barrio-porteno-que-concentra-las-quejas-por-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1436,7 +1436,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/dolar/dolar-hoy-dolar-blue-hoy-a-cuanto-cotiza-este-jueves-3-de-abril-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/cultura/el-gobierno-no-le-renovo-el-contrato-al-fotografo-que-saco-la-foto-al-cabo-que-hirio-a-pablo-grillo-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1446,7 +1446,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/festejo-a-lo-grande-asi-se-celebraron-los-70-anos-de-fabrica-santa-isabel-de-renault-la-primera-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/sociedad/caos-en-palermo-por-el-show-gratuito-de-tini-stoessel-peleas-entre-fanaticas-y-quejas-de-los-vecinos-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1456,7 +1456,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/deportes/tenis/el-expreparador-fisico-de-sinner-demonizado-por-haber-comprado-la-sustancia-prohibida-le-apunto-al-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/festejo-a-lo-grande-asi-se-celebraron-los-70-anos-de-fabrica-santa-isabel-de-renault-la-primera-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1466,7 +1466,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/</t>
+          <t>https://www.lanacion.com.ar/deportes/tenis/el-expreparador-fisico-de-sinner-demonizado-por-haber-comprado-la-sustancia-prohibida-le-apunto-al-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/negocios/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/</t>
         </is>
       </c>
     </row>
@@ -1486,7 +1486,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/</t>
+          <t>https://www.lanacion.com.ar/economia/negocios/</t>
         </is>
       </c>
     </row>
@@ -1496,7 +1496,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/milei-se-reunio-con-el-presidente-del-banco-mundial-quien-destaco-que-trabaja-en-un-paquete-de-apoyo-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/propiedades/</t>
         </is>
       </c>
     </row>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/foro-llao-llao-sin-candidatos-ni-funcionarios-comenzo-la-decima-edicion-del-encuentro-que-reune-a-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/economia/milei-se-reunio-con-el-presidente-del-banco-mundial-quien-destaco-que-trabaja-en-un-paquete-de-apoyo-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/negocios/cadenas-de-oro-las-acciones-y-el-dilema-de-los-ejecutivos-nid29032025/</t>
+          <t>https://www.lanacion.com.ar/economia/foro-llao-llao-sin-candidatos-ni-funcionarios-comenzo-la-decima-edicion-del-encuentro-que-reune-a-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1526,7 +1526,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/negocios/el-cafe-argentino-que-se-destaca-en-un-famoso-barrio-madrileno-nid27032025/</t>
+          <t>https://www.lanacion.com.ar/economia/negocios/cadenas-de-oro-las-acciones-y-el-dilema-de-los-ejecutivos-nid29032025/</t>
         </is>
       </c>
     </row>
@@ -1536,7 +1536,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/mauro-francisco-protagoniza-en-calle-corrientes-pero-se-niega-a-abandonar-su-empleo-como-chofer-de-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/economia/negocios/el-cafe-argentino-que-se-destaca-en-un-famoso-barrio-madrileno-nid27032025/</t>
         </is>
       </c>
     </row>
@@ -1546,7 +1546,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/musica/quilmes-rock-2025-lo-que-hay-que-saber-del-festival-que-comienza-el-sabado-y-del-documental-que-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/mauro-francisco-protagoniza-en-calle-corrientes-pero-se-niega-a-abandonar-su-empleo-como-chofer-de-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1556,7 +1556,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/personajes/postrado-en-una-cama-y-casi-sin-voz-asi-vivio-val-kilmer-sus-ultimos-anos-de-vida-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/musica/quilmes-rock-2025-lo-que-hay-que-saber-del-festival-que-comienza-el-sabado-y-del-documental-que-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1566,7 +1566,7 @@
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/que-sale/de-narda-lepes-a-betular-quienes-son-los-mas-de-40-reconocidos-chefs-que-cocinaran-por-bahia-blanca-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/espectaculos/personajes/postrado-en-una-cama-y-casi-sin-voz-asi-vivio-val-kilmer-sus-ultimos-anos-de-vida-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1576,7 +1576,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/que-sale/tapeando-2025-el-mapa-con-los-restaurantes-que-ofrecen-tapas-a-precios-especiales-nid19032025/</t>
+          <t>https://www.lanacion.com.ar/que-sale/de-narda-lepes-a-betular-quienes-son-los-mas-de-40-reconocidos-chefs-que-cocinaran-por-bahia-blanca-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1586,7 +1586,7 @@
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/sabado/el-bodegon-que-le-devolvio-su-identidad-al-bajo-de-san-isidro-nid28032025/</t>
+          <t>https://www.lanacion.com.ar/que-sale/tapeando-2025-el-mapa-con-los-restaurantes-que-ofrecen-tapas-a-precios-especiales-nid19032025/</t>
         </is>
       </c>
     </row>
@@ -1596,7 +1596,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/que-sale/el-eternauta-en-netflix-cuando-se-estrena-la-serie-con-ricardo-darin-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/sabado/el-bodegon-que-le-devolvio-su-identidad-al-bajo-de-san-isidro-nid28032025/</t>
         </is>
       </c>
     </row>
@@ -1606,7 +1606,7 @@
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/vida_sana/</t>
+          <t>https://www.lanacion.com.ar/que-sale/el-eternauta-en-netflix-cuando-se-estrena-la-serie-con-ricardo-darin-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1616,7 +1616,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/nutricion/</t>
+          <t>https://www.lanacion.com.ar/salud/vida_sana/</t>
         </is>
       </c>
     </row>
@@ -1626,7 +1626,7 @@
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/fitness/</t>
+          <t>https://www.lanacion.com.ar/salud/nutricion/</t>
         </is>
       </c>
     </row>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/mente/</t>
+          <t>https://www.lanacion.com.ar/salud/fitness/</t>
         </is>
       </c>
     </row>
@@ -1646,7 +1646,7 @@
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/descanso/</t>
+          <t>https://www.lanacion.com.ar/salud/mente/</t>
         </is>
       </c>
     </row>
@@ -1656,7 +1656,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/turismo/viajes/</t>
+          <t>https://www.lanacion.com.ar/salud/descanso/</t>
         </is>
       </c>
     </row>
@@ -1666,7 +1666,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/nutricion/ni-manzana-ni-cereza-la-joya-roja-que-estimula-el-colageno-naturalmente-y-ya-se-cultiva-en-el-pais-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/turismo/viajes/</t>
         </is>
       </c>
     </row>
@@ -1676,7 +1676,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/las-mejores-piscinas-naturales-del-nordeste-de-brasil-para-nadar-entre-peces-de-colores-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/salud/nutricion/ni-manzana-ni-cereza-la-joya-roja-que-estimula-el-colageno-naturalmente-y-ya-se-cultiva-en-el-pais-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1686,7 +1686,7 @@
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/mente/ni-casados-ni-solteros-agamia-el-fenomeno-que-gana-terreno-entre-los-jovenes-nid31032025/</t>
+          <t>https://www.lanacion.com.ar/salud/las-mejores-piscinas-naturales-del-nordeste-de-brasil-para-nadar-entre-peces-de-colores-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1696,7 +1696,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/salud/nutricion/un-especialista-explica-que-ocurre-cuando-se-consume-vitamina-d-y-magnesio-al-mismo-tiempo-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/salud/mente/ni-casados-ni-solteros-agamia-el-fenomeno-que-gana-terreno-entre-los-jovenes-nid31032025/</t>
         </is>
       </c>
     </row>
@@ -1706,7 +1706,7 @@
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/tendencias/</t>
+          <t>https://www.lanacion.com.ar/salud/nutricion/un-especialista-explica-que-ocurre-cuando-se-consume-vitamina-d-y-magnesio-al-mismo-tiempo-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1716,7 +1716,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/test-drive/</t>
+          <t>https://www.lanacion.com.ar/autos/tendencias/</t>
         </is>
       </c>
     </row>
@@ -1726,7 +1726,7 @@
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/electricos/</t>
+          <t>https://www.lanacion.com.ar/autos/test-drive/</t>
         </is>
       </c>
     </row>
@@ -1736,7 +1736,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/manejaba-a-16kmh-lo-multaron-por-exceso-de-velocidad-y-cambio-el-destino-de-su-empresa-para-siempre-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/autos/electricos/</t>
         </is>
       </c>
     </row>
@@ -1746,7 +1746,7 @@
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/vtv-estos-son-los-cuatro-errores-mas-comunes-de-quienes-no-pasan-la-revision-nid01042025/</t>
+          <t>https://www.lanacion.com.ar/autos/manejaba-a-16kmh-lo-multaron-por-exceso-de-velocidad-y-cambio-el-destino-de-su-empresa-para-siempre-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1756,7 +1756,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/las-fabricas-de-autos-del-futuro-y-el-desafio-chino-como-se-preparan-las-automotrices-para-la-nueva-nid01042025/</t>
+          <t>https://www.lanacion.com.ar/autos/vtv-estos-son-los-cuatro-errores-mas-comunes-de-quienes-no-pasan-la-revision-nid01042025/</t>
         </is>
       </c>
     </row>
@@ -1766,7 +1766,7 @@
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/autos/una-pickup-volvio-a-ser-la-mas-vendida-y-los-patentamientos-de-autos-cerraron-el-mejor-primer-nid31032025/</t>
+          <t>https://www.lanacion.com.ar/autos/las-fabricas-de-autos-del-futuro-y-el-desafio-chino-como-se-preparan-las-automotrices-para-la-nueva-nid01042025/</t>
         </is>
       </c>
     </row>
@@ -1776,7 +1776,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/</t>
+          <t>https://www.lanacion.com.ar/autos/una-pickup-volvio-a-ser-la-mas-vendida-y-los-patentamientos-de-autos-cerraron-el-mejor-primer-nid31032025/</t>
         </is>
       </c>
     </row>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/construccion-y-diseno/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/</t>
         </is>
       </c>
     </row>
@@ -1796,7 +1796,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/inmuebles-comerciales/</t>
+          <t>https://www.lanacion.com.ar/propiedades/construccion-y-diseno/</t>
         </is>
       </c>
     </row>
@@ -1806,7 +1806,7 @@
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/inversiones/</t>
+          <t>https://www.lanacion.com.ar/propiedades/inmuebles-comerciales/</t>
         </is>
       </c>
     </row>
@@ -1816,7 +1816,7 @@
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/creditos-hipotecarios-cuanto-hay-que-ganar-para-comprar-un-departamento-nid01042025/</t>
+          <t>https://www.lanacion.com.ar/propiedades/inversiones/</t>
         </is>
       </c>
     </row>
@@ -1826,7 +1826,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/construccion-y-diseno/el-invento-que-promete-revolucionar-la-construccion-levantar-paredes-sin-cemento-y-con-piezas-que-nid01042025/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/creditos-hipotecarios-cuanto-hay-que-ganar-para-comprar-un-departamento-nid01042025/</t>
         </is>
       </c>
     </row>
@@ -1836,7 +1836,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/este-es-el-barrio-con-los-alquileres-mas-baratos-en-caba-en-abril-2025-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/propiedades/construccion-y-diseno/el-invento-que-promete-revolucionar-la-construccion-levantar-paredes-sin-cemento-y-con-piezas-que-nid01042025/</t>
         </is>
       </c>
     </row>
@@ -1846,7 +1846,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/los-metodos-faciles-para-calcular-el-aumento-del-alquiler-en-abril-2025-nid01042025/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/este-es-el-barrio-con-los-alquileres-mas-baratos-en-caba-en-abril-2025-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1856,7 +1856,7 @@
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/agricultura/</t>
+          <t>https://www.lanacion.com.ar/propiedades/casas-y-departamentos/los-metodos-faciles-para-calcular-el-aumento-del-alquiler-en-abril-2025-nid01042025/</t>
         </is>
       </c>
     </row>
@@ -1866,7 +1866,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/ganaderia/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/agricultura/</t>
         </is>
       </c>
     </row>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/tecnologias/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/ganaderia/</t>
         </is>
       </c>
     </row>
@@ -1886,7 +1886,7 @@
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/regionales/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/tecnologias/</t>
         </is>
       </c>
     </row>
@@ -1896,7 +1896,7 @@
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/oportunidad-estrategica-facturo-us1242-millones-una-joya-del-mercado-que-no-para-de-crecer-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/regionales/</t>
         </is>
       </c>
     </row>
@@ -1906,7 +1906,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/escenario-excelente-tras-las-politicas-populistas-lo-que-viene-para-la-ganaderia-son-inversiones-y-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/oportunidad-estrategica-facturo-us1242-millones-una-joya-del-mercado-que-no-para-de-crecer-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1916,7 +1916,7 @@
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/emprendedor-condujo-a-40-soldados-en-malvinas-y-en-la-guerra-vio-un-animal-con-el-cual-hoy-vive-un-nid02042024/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/escenario-excelente-tras-las-politicas-populistas-lo-que-viene-para-la-ganaderia-son-inversiones-y-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1926,7 +1926,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/economia/campo/chicos-jugando-a-ser-soldados-fue-a-combatir-a-malvinas-se-salvo-de-milagro-y-hoy-en-un-lugar-unico-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/emprendedor-condujo-a-40-soldados-en-malvinas-y-en-la-guerra-vio-un-animal-con-el-cual-hoy-vive-un-nid02042024/</t>
         </is>
       </c>
     </row>
@@ -1936,7 +1936,7 @@
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/llego-negada-a-eeuu-logro-cosas-increibles-y-cuenta-el-lado-a-y-b-de-nueva-york-dejar-la-queja-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/economia/campo/chicos-jugando-a-ser-soldados-fue-a-combatir-a-malvinas-se-salvo-de-milagro-y-hoy-en-un-lugar-unico-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1946,7 +1946,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/esgrima-de-cuchillo-entre-el-facon-gauchesco-las-referencias-borgeanas-y-la-supervivencia-barrial-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/llego-negada-a-eeuu-logro-cosas-increibles-y-cuenta-el-lado-a-y-b-de-nueva-york-dejar-la-queja-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1956,7 +1956,7 @@
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/lifestyle/tapeando-para-los-amantes-de-las-tapas-un-recorrido-posible-para-celebrar-la-tradicion-espanola-a-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/esgrima-de-cuchillo-entre-el-facon-gauchesco-las-referencias-borgeanas-y-la-supervivencia-barrial-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1966,7 +1966,7 @@
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-living/una-casa-de-pueblo-que-hoy-es-un-icono-nid02042025/</t>
+          <t>https://www.lanacion.com.ar/lifestyle/tapeando-para-los-amantes-de-las-tapas-un-recorrido-posible-para-celebrar-la-tradicion-espanola-a-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -1976,7 +1976,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/revista-living/llega-experiencia-living-la-muestra-de-diseno-del-ano-que-no-te-podes-perder-nid31032025/</t>
+          <t>https://www.lanacion.com.ar/revista-living/una-casa-de-pueblo-que-hoy-es-un-icono-nid02042025/</t>
         </is>
       </c>
     </row>
@@ -1986,7 +1986,7 @@
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/loterias/ganaron-mas-de-840-millones-en-el-quini-6-cuales-fueron-los-numeros-de-la-suerte-del-sorteo-del-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/revista-living/llega-experiencia-living-la-muestra-de-diseno-del-ano-que-no-te-podes-perder-nid31032025/</t>
         </is>
       </c>
     </row>
@@ -1996,7 +1996,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/politica/calendario-de-elecciones-2025-provincia-por-provincia-cuando-se-vota-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/loterias/ganaron-mas-de-840-millones-en-el-quini-6-cuales-fueron-los-numeros-de-la-suerte-del-sorteo-del-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -2006,7 +2006,7 @@
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>https://www.lanacion.com.ar/espectaculos/como-ver-el-quilmes-rock-2025-en-vivo-nid03042025/</t>
+          <t>https://www.lanacion.com.ar/politica/calendario-de-elecciones-2025-provincia-por-provincia-cuando-se-vota-nid03042025/</t>
         </is>
       </c>
     </row>
@@ -2015,6 +2015,16 @@
         <v>157</v>
       </c>
       <c r="B159" t="inlineStr">
+        <is>
+          <t>https://www.lanacion.com.ar/espectaculos/como-ver-el-quilmes-rock-2025-en-vivo-nid03042025/</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" s="1" t="n">
+        <v>158</v>
+      </c>
+      <c r="B160" t="inlineStr">
         <is>
           <t>https://www.lanacion.com.ar/feriados/2025/cuando-es-el-proximo-feriado-de-abril-2025-nid02042025/</t>
         </is>

</xml_diff>